<commit_message>
add 4 feilds to employee
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emad/projects/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63233F22-8719-0C4D-A7B4-E3F5709A69F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEBF832-C42D-F14C-BD5B-B645570D83E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="23600" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="30260" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="161">
   <si>
     <t>name</t>
   </si>
@@ -479,12 +479,39 @@
   </si>
   <si>
     <t>موظف ١٠</t>
+  </si>
+  <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>currentJob</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Nipal</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,11 +570,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,19 +883,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,46 +934,58 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -942,47 +1004,59 @@
       <c r="F2" t="s">
         <v>51</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="3">
+        <v>38900</v>
+      </c>
+      <c r="I2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2">
         <v>5452</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>1059</v>
       </c>
-      <c r="I2">
+      <c r="M2">
         <v>6511</v>
       </c>
-      <c r="J2">
+      <c r="N2">
         <v>27.13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>61</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>81</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>101</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>118</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1001,47 +1075,59 @@
       <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="3">
+        <v>38726</v>
+      </c>
+      <c r="I3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3">
         <v>3840</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>636</v>
       </c>
-      <c r="I3">
+      <c r="M3">
         <v>4476</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>18.649999999999999</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>62</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>82</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
         <v>102</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>119</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="S3" t="s">
+      <c r="W3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1060,47 +1146,59 @@
       <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="3">
+        <v>38847</v>
+      </c>
+      <c r="I4" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" t="s">
+        <v>157</v>
+      </c>
+      <c r="K4">
         <v>5328</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>1338</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>6666</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>27.77</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>83</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>103</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>120</v>
       </c>
-      <c r="R4" t="s">
+      <c r="V4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1119,47 +1217,59 @@
       <c r="F5" t="s">
         <v>54</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="3">
+        <v>38467</v>
+      </c>
+      <c r="I5" t="s">
+        <v>160</v>
+      </c>
+      <c r="J5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5">
         <v>4800</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>2501</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <v>7301</v>
       </c>
-      <c r="J5">
+      <c r="N5">
         <v>30.42</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>64</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>84</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S5" t="s">
         <v>104</v>
       </c>
-      <c r="P5" t="s">
+      <c r="T5" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="U5" t="s">
         <v>121</v>
       </c>
-      <c r="R5" t="s">
+      <c r="V5" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="S5" t="s">
+      <c r="W5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1178,47 +1288,59 @@
       <c r="F6" t="s">
         <v>55</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="3">
+        <v>39373</v>
+      </c>
+      <c r="I6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K6">
         <v>2657</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>1104</v>
       </c>
-      <c r="I6">
+      <c r="M6">
         <v>3761</v>
       </c>
-      <c r="J6">
+      <c r="N6">
         <v>15.67</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>65</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>85</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O6" t="s">
+      <c r="S6" t="s">
         <v>105</v>
       </c>
-      <c r="P6" t="s">
+      <c r="T6" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="U6" t="s">
         <v>122</v>
       </c>
-      <c r="R6" t="s">
+      <c r="V6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="S6" t="s">
+      <c r="W6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1237,47 +1359,59 @@
       <c r="F7" t="s">
         <v>56</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="3">
+        <v>38778</v>
+      </c>
+      <c r="I7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K7">
         <v>3512</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>1728</v>
       </c>
-      <c r="I7">
+      <c r="M7">
         <v>5240</v>
       </c>
-      <c r="J7">
+      <c r="N7">
         <v>21.83</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>66</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>86</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O7" t="s">
+      <c r="S7" t="s">
         <v>106</v>
       </c>
-      <c r="P7" t="s">
+      <c r="T7" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="U7" t="s">
         <v>123</v>
       </c>
-      <c r="R7" t="s">
+      <c r="V7" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="S7" t="s">
+      <c r="W7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1296,47 +1430,59 @@
       <c r="F8" t="s">
         <v>57</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="3">
+        <v>38646</v>
+      </c>
+      <c r="I8" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8">
         <v>3377</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>1830</v>
       </c>
-      <c r="I8">
+      <c r="M8">
         <v>5207</v>
       </c>
-      <c r="J8">
+      <c r="N8">
         <v>21.7</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O8" t="s">
         <v>67</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q8" t="s">
         <v>87</v>
       </c>
-      <c r="N8" t="s">
+      <c r="R8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="O8" t="s">
+      <c r="S8" t="s">
         <v>107</v>
       </c>
-      <c r="P8" t="s">
+      <c r="T8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="U8" t="s">
         <v>124</v>
       </c>
-      <c r="R8" t="s">
+      <c r="V8" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="S8" t="s">
+      <c r="W8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1355,47 +1501,59 @@
       <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="3">
+        <v>39242</v>
+      </c>
+      <c r="I9" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K9">
         <v>2759</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>2138</v>
       </c>
-      <c r="I9">
+      <c r="M9">
         <v>4897</v>
       </c>
-      <c r="J9">
+      <c r="N9">
         <v>20.399999999999999</v>
       </c>
-      <c r="K9" t="s">
+      <c r="O9" t="s">
         <v>68</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
         <v>88</v>
       </c>
-      <c r="N9" t="s">
+      <c r="R9" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="O9" t="s">
+      <c r="S9" t="s">
         <v>108</v>
       </c>
-      <c r="P9" t="s">
+      <c r="T9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="U9" t="s">
         <v>125</v>
       </c>
-      <c r="R9" t="s">
+      <c r="V9" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="S9" t="s">
+      <c r="W9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1414,47 +1572,59 @@
       <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H10" s="3">
+        <v>38973</v>
+      </c>
+      <c r="I10" t="s">
+        <v>160</v>
+      </c>
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10">
         <v>6399</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>1181</v>
       </c>
-      <c r="I10">
+      <c r="M10">
         <v>7580</v>
       </c>
-      <c r="J10">
+      <c r="N10">
         <v>31.58</v>
       </c>
-      <c r="K10" t="s">
+      <c r="O10" t="s">
         <v>69</v>
       </c>
-      <c r="L10" t="s">
+      <c r="P10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M10" t="s">
+      <c r="Q10" t="s">
         <v>89</v>
       </c>
-      <c r="N10" t="s">
+      <c r="R10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="O10" t="s">
+      <c r="S10" t="s">
         <v>109</v>
       </c>
-      <c r="P10" t="s">
+      <c r="T10" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="U10" t="s">
         <v>126</v>
       </c>
-      <c r="R10" t="s">
+      <c r="V10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="S10" t="s">
+      <c r="W10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1473,43 +1643,55 @@
       <c r="F11" t="s">
         <v>60</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="s">
+        <v>158</v>
+      </c>
+      <c r="H11" s="3">
+        <v>38310</v>
+      </c>
+      <c r="I11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" t="s">
+        <v>157</v>
+      </c>
+      <c r="K11">
         <v>7350</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>2488</v>
       </c>
-      <c r="I11">
+      <c r="M11">
         <v>9838</v>
       </c>
-      <c r="J11">
+      <c r="N11">
         <v>40.99</v>
       </c>
-      <c r="K11" t="s">
+      <c r="O11" t="s">
         <v>70</v>
       </c>
-      <c r="L11" t="s">
+      <c r="P11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>90</v>
       </c>
-      <c r="N11" t="s">
+      <c r="R11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="O11" t="s">
+      <c r="S11" t="s">
         <v>110</v>
       </c>
-      <c r="P11" t="s">
+      <c r="T11" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="U11" t="s">
         <v>127</v>
       </c>
-      <c r="R11" t="s">
+      <c r="V11" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="S11" t="s">
+      <c r="W11" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>